<commit_message>
TST: Test for float --> int in the middle of object dtype
</commit_message>
<xml_diff>
--- a/pandas/io/tests/data/test_types.xlsx
+++ b/pandas/io/tests/data/test_types.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="6200" yWindow="2220" windowWidth="25600" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>IntCol</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
   </si>
   <si>
     <t>c</t>
@@ -443,7 +440,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -468,7 +465,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -504,8 +501,8 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
+      <c r="E3">
+        <v>3</v>
       </c>
       <c r="F3" s="2">
         <v>41578</v>
@@ -525,7 +522,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2">
         <v>1828</v>
@@ -545,7 +542,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2">
         <v>41622</v>
@@ -565,7 +562,7 @@
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2">
         <v>42077</v>

</xml_diff>